<commit_message>
Update flume tank data
</commit_message>
<xml_diff>
--- a/analysis/flume_tank/data/flume_tank_data.xlsx
+++ b/analysis/flume_tank/data/flume_tank_data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="88">
   <si>
     <t>date_time_nst</t>
   </si>
@@ -677,7 +677,6 @@
   <cols>
     <col hidden="1" min="1" max="1" width="12.63"/>
     <col customWidth="1" min="15" max="15" width="16.75"/>
-    <col hidden="1" min="16" max="18" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -934,7 +933,7 @@
         <v>2.0</v>
       </c>
       <c r="U3" s="4">
-        <v>68.2</v>
+        <v>74.0</v>
       </c>
       <c r="V3" s="2">
         <v>17.5</v>
@@ -969,7 +968,7 @@
       </c>
       <c r="AJ3" s="6"/>
       <c r="AK3" s="4">
-        <v>11.0</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="4">
@@ -1030,7 +1029,7 @@
         <v>2.5</v>
       </c>
       <c r="U4" s="4">
-        <v>64.5</v>
+        <v>69.8</v>
       </c>
       <c r="V4" s="2">
         <v>17.5</v>
@@ -1065,7 +1064,7 @@
       </c>
       <c r="AJ4" s="6"/>
       <c r="AK4" s="4">
-        <v>10.0</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="5">
@@ -1126,7 +1125,7 @@
         <v>3.0</v>
       </c>
       <c r="U5" s="4">
-        <v>64.6</v>
+        <v>70.0</v>
       </c>
       <c r="V5" s="2">
         <v>17.5</v>
@@ -1162,7 +1161,7 @@
       </c>
       <c r="AJ5" s="6"/>
       <c r="AK5" s="4">
-        <v>10.3</v>
+        <v>20.8</v>
       </c>
     </row>
     <row r="6">
@@ -1223,7 +1222,7 @@
         <v>3.5</v>
       </c>
       <c r="U6" s="4">
-        <v>66.4</v>
+        <v>72.0</v>
       </c>
       <c r="V6" s="2">
         <v>17.5</v>
@@ -1259,7 +1258,7 @@
       </c>
       <c r="AJ6" s="6"/>
       <c r="AK6" s="4">
-        <v>10.6</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="7">
@@ -1320,7 +1319,7 @@
         <v>4.0</v>
       </c>
       <c r="U7" s="4">
-        <v>66.4</v>
+        <v>72.0</v>
       </c>
       <c r="V7" s="2">
         <v>17.5</v>
@@ -1356,7 +1355,7 @@
       </c>
       <c r="AJ7" s="6"/>
       <c r="AK7" s="4">
-        <v>10.6</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="8">
@@ -1417,7 +1416,7 @@
         <v>3.0</v>
       </c>
       <c r="U8" s="4">
-        <v>64.6</v>
+        <v>70.0</v>
       </c>
       <c r="V8" s="2">
         <v>17.5</v>
@@ -1453,7 +1452,7 @@
       </c>
       <c r="AJ8" s="6"/>
       <c r="AK8" s="4">
-        <v>10.3</v>
+        <v>20.8</v>
       </c>
     </row>
     <row r="9">
@@ -1510,7 +1509,7 @@
         <v>3.0</v>
       </c>
       <c r="U9" s="4">
-        <v>75.9</v>
+        <v>88.0</v>
       </c>
       <c r="V9" s="2">
         <v>20.0</v>
@@ -1542,7 +1541,7 @@
       </c>
       <c r="AJ9" s="6"/>
       <c r="AK9" s="4">
-        <v>12.2</v>
+        <v>30.7</v>
       </c>
     </row>
     <row r="10">
@@ -1603,7 +1602,7 @@
         <v>3.0</v>
       </c>
       <c r="U10" s="4">
-        <v>34.4</v>
+        <v>37.0</v>
       </c>
       <c r="V10" s="2">
         <v>12.5</v>
@@ -1639,7 +1638,7 @@
       </c>
       <c r="AJ10" s="6"/>
       <c r="AK10" s="4">
-        <v>4.9</v>
+        <v>9.8</v>
       </c>
     </row>
     <row r="11">
@@ -1700,7 +1699,7 @@
         <v>3.5</v>
       </c>
       <c r="U11" s="4">
-        <v>34.2</v>
+        <v>36.8</v>
       </c>
       <c r="V11" s="2">
         <v>12.5</v>
@@ -1736,7 +1735,7 @@
       </c>
       <c r="AJ11" s="6"/>
       <c r="AK11" s="4">
-        <v>4.9</v>
+        <v>9.8</v>
       </c>
     </row>
     <row r="12">
@@ -1795,7 +1794,7 @@
         <v>2.5</v>
       </c>
       <c r="U12" s="4">
-        <v>35.5</v>
+        <v>38.2</v>
       </c>
       <c r="V12" s="2">
         <v>12.5</v>
@@ -1831,7 +1830,7 @@
       </c>
       <c r="AJ12" s="6"/>
       <c r="AK12" s="4">
-        <v>5.1</v>
+        <v>10.2</v>
       </c>
     </row>
     <row r="13">
@@ -1888,7 +1887,7 @@
         <v>3.0</v>
       </c>
       <c r="U13" s="4">
-        <v>66.5</v>
+        <v>72.1</v>
       </c>
       <c r="V13" s="2">
         <v>17.5</v>
@@ -1925,7 +1924,7 @@
         <v>61.1</v>
       </c>
       <c r="AK13" s="4">
-        <v>10.7</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="14">
@@ -1982,7 +1981,7 @@
         <v>3.0</v>
       </c>
       <c r="U14" s="4">
-        <v>66.5</v>
+        <v>72.1</v>
       </c>
       <c r="V14" s="2">
         <v>17.5</v>
@@ -2025,7 +2024,7 @@
         <v>68.9</v>
       </c>
       <c r="AK14" s="4">
-        <v>10.8</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="15">
@@ -2082,7 +2081,7 @@
         <v>3.0</v>
       </c>
       <c r="U15" s="4">
-        <v>66.5</v>
+        <v>72.1</v>
       </c>
       <c r="V15" s="2">
         <v>17.5</v>
@@ -2126,7 +2125,7 @@
         <v>70.0</v>
       </c>
       <c r="AK15" s="4">
-        <v>10.7</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="16">
@@ -2183,7 +2182,7 @@
         <v>2.5</v>
       </c>
       <c r="U16" s="4">
-        <v>74.5</v>
+        <v>86.3</v>
       </c>
       <c r="V16" s="2">
         <v>20.0</v>
@@ -2218,7 +2217,7 @@
       </c>
       <c r="AJ16" s="6"/>
       <c r="AK16" s="4">
-        <v>11.9</v>
+        <v>29.9</v>
       </c>
     </row>
     <row r="17">
@@ -2275,7 +2274,7 @@
         <v>3.5</v>
       </c>
       <c r="U17" s="4">
-        <v>77.7</v>
+        <v>90.2</v>
       </c>
       <c r="V17" s="2">
         <v>20.0</v>
@@ -2311,7 +2310,7 @@
       </c>
       <c r="AJ17" s="6"/>
       <c r="AK17" s="4">
-        <v>12.6</v>
+        <v>31.9</v>
       </c>
     </row>
     <row r="18">
@@ -2370,7 +2369,7 @@
         <v>2.0</v>
       </c>
       <c r="U18" s="4">
-        <v>70.2</v>
+        <v>74.0</v>
       </c>
       <c r="V18" s="2">
         <v>17.5</v>
@@ -2413,7 +2412,7 @@
         <v>24.7</v>
       </c>
       <c r="AK18" s="4">
-        <v>14.8</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="19">
@@ -2472,7 +2471,7 @@
         <v>2.5</v>
       </c>
       <c r="U19" s="4">
-        <v>68.3</v>
+        <v>72.0</v>
       </c>
       <c r="V19" s="2">
         <v>17.5</v>
@@ -2516,7 +2515,7 @@
         <v>42.7</v>
       </c>
       <c r="AK19" s="4">
-        <v>14.3</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="20">
@@ -2575,7 +2574,7 @@
         <v>3.0</v>
       </c>
       <c r="U20" s="4">
-        <v>68.3</v>
+        <v>72.1</v>
       </c>
       <c r="V20" s="2">
         <v>17.5</v>
@@ -2619,7 +2618,7 @@
         <v>68.9</v>
       </c>
       <c r="AK20" s="4">
-        <v>14.3</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="21">
@@ -2678,7 +2677,7 @@
         <v>3.5</v>
       </c>
       <c r="U21" s="4">
-        <v>68.3</v>
+        <v>72.0</v>
       </c>
       <c r="V21" s="2">
         <v>17.5</v>
@@ -2722,7 +2721,7 @@
         <v>103.7</v>
       </c>
       <c r="AK21" s="4">
-        <v>14.3</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="22">
@@ -2781,7 +2780,7 @@
         <v>4.0</v>
       </c>
       <c r="U22" s="4">
-        <v>68.3</v>
+        <v>72.1</v>
       </c>
       <c r="V22" s="2">
         <v>17.5</v>
@@ -2825,7 +2824,7 @@
         <v>142.8</v>
       </c>
       <c r="AK22" s="4">
-        <v>14.3</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="23">
@@ -2884,7 +2883,7 @@
         <v>3.0</v>
       </c>
       <c r="U23" s="4">
-        <v>68.4</v>
+        <v>72.1</v>
       </c>
       <c r="V23" s="2">
         <v>17.5</v>
@@ -2928,7 +2927,7 @@
         <v>67.9</v>
       </c>
       <c r="AK23" s="4">
-        <v>14.4</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="24">
@@ -2987,7 +2986,7 @@
         <v>3.0</v>
       </c>
       <c r="U24" s="4">
-        <v>68.4</v>
+        <v>72.2</v>
       </c>
       <c r="V24" s="2">
         <v>17.5</v>
@@ -3031,7 +3030,7 @@
         <v>64.6</v>
       </c>
       <c r="AK24" s="4">
-        <v>14.5</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="25">
@@ -3090,7 +3089,7 @@
         <v>3.0</v>
       </c>
       <c r="U25" s="4">
-        <v>68.5</v>
+        <v>72.3</v>
       </c>
       <c r="V25" s="2">
         <v>17.5</v>
@@ -3134,7 +3133,7 @@
         <v>62.1</v>
       </c>
       <c r="AK25" s="4">
-        <v>14.6</v>
+        <v>22.1</v>
       </c>
     </row>
     <row r="26">
@@ -3193,7 +3192,7 @@
         <v>2.5</v>
       </c>
       <c r="U26" s="4">
-        <v>36.4</v>
+        <v>38.3</v>
       </c>
       <c r="V26" s="2">
         <v>12.5</v>
@@ -3236,7 +3235,7 @@
         <v>42.2</v>
       </c>
       <c r="AK26" s="4">
-        <v>6.9</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="27">
@@ -3295,7 +3294,7 @@
         <v>3.0</v>
       </c>
       <c r="U27" s="4">
-        <v>35.5</v>
+        <v>37.3</v>
       </c>
       <c r="V27" s="2">
         <v>12.5</v>
@@ -3339,7 +3338,7 @@
         <v>69.2</v>
       </c>
       <c r="AK27" s="4">
-        <v>6.6</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="28">
@@ -3398,7 +3397,7 @@
         <v>3.5</v>
       </c>
       <c r="U28" s="4">
-        <v>34.6</v>
+        <v>36.3</v>
       </c>
       <c r="V28" s="2">
         <v>12.5</v>
@@ -3442,7 +3441,7 @@
         <v>107.9</v>
       </c>
       <c r="AK28" s="4">
-        <v>6.4</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="29">
@@ -3501,7 +3500,7 @@
         <v>3.0</v>
       </c>
       <c r="U29" s="4">
-        <v>66.5</v>
+        <v>70.1</v>
       </c>
       <c r="V29" s="2">
         <v>17.5</v>
@@ -3537,7 +3536,7 @@
       </c>
       <c r="AJ29" s="6"/>
       <c r="AK29" s="4">
-        <v>13.8</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="30">
@@ -3596,7 +3595,7 @@
         <v>3.0</v>
       </c>
       <c r="U30" s="4">
-        <v>66.4</v>
+        <v>70.0</v>
       </c>
       <c r="V30" s="2">
         <v>17.5</v>
@@ -3632,7 +3631,7 @@
       </c>
       <c r="AJ30" s="6"/>
       <c r="AK30" s="4">
-        <v>13.7</v>
+        <v>20.8</v>
       </c>
     </row>
     <row r="31">
@@ -3691,7 +3690,7 @@
         <v>3.0</v>
       </c>
       <c r="U31" s="4">
-        <v>66.4</v>
+        <v>70.0</v>
       </c>
       <c r="V31" s="2">
         <v>17.5</v>
@@ -3727,7 +3726,7 @@
       </c>
       <c r="AJ31" s="6"/>
       <c r="AK31" s="4">
-        <v>13.8</v>
+        <v>20.8</v>
       </c>
     </row>
     <row r="32">
@@ -3786,7 +3785,7 @@
         <v>2.5</v>
       </c>
       <c r="U32" s="4">
-        <v>142.1</v>
+        <v>109.0</v>
       </c>
       <c r="V32" s="2">
         <v>20.0</v>
@@ -3889,7 +3888,7 @@
         <v>3.0</v>
       </c>
       <c r="U33" s="4">
-        <v>142.3</v>
+        <v>109.1</v>
       </c>
       <c r="V33" s="2">
         <v>20.0</v>
@@ -3992,7 +3991,7 @@
         <v>3.5</v>
       </c>
       <c r="U34" s="4">
-        <v>142.5</v>
+        <v>109.2</v>
       </c>
       <c r="V34" s="2">
         <v>20.0</v>
@@ -4095,7 +4094,7 @@
         <v>3.0</v>
       </c>
       <c r="U35" s="4">
-        <v>103.6</v>
+        <v>80.2</v>
       </c>
       <c r="V35" s="2">
         <v>17.5</v>
@@ -4448,7 +4447,7 @@
         <v>2.0</v>
       </c>
       <c r="U39" s="4">
-        <v>55.8</v>
+        <v>60.4</v>
       </c>
       <c r="V39" s="2">
         <v>16.0</v>
@@ -4495,7 +4494,7 @@
         <v>22.0</v>
       </c>
       <c r="AK39" s="4">
-        <v>8.7</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="40">
@@ -4552,7 +4551,7 @@
         <v>2.5</v>
       </c>
       <c r="U40" s="4">
-        <v>55.8</v>
+        <v>60.5</v>
       </c>
       <c r="V40" s="2">
         <v>16.0</v>
@@ -4599,7 +4598,7 @@
         <v>35.0</v>
       </c>
       <c r="AK40" s="4">
-        <v>8.8</v>
+        <v>17.7</v>
       </c>
     </row>
     <row r="41">
@@ -4656,7 +4655,7 @@
         <v>3.0</v>
       </c>
       <c r="U41" s="4">
-        <v>55.9</v>
+        <v>60.5</v>
       </c>
       <c r="V41" s="2">
         <v>16.0</v>
@@ -4703,7 +4702,7 @@
         <v>54.0</v>
       </c>
       <c r="AK41" s="4">
-        <v>8.8</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="42">
@@ -4760,7 +4759,7 @@
         <v>3.5</v>
       </c>
       <c r="U42" s="4">
-        <v>55.9</v>
+        <v>60.5</v>
       </c>
       <c r="V42" s="2">
         <v>16.0</v>
@@ -4807,7 +4806,7 @@
         <v>82.0</v>
       </c>
       <c r="AK42" s="4">
-        <v>8.8</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="43">
@@ -4864,7 +4863,7 @@
         <v>4.0</v>
       </c>
       <c r="U43" s="4">
-        <v>55.9</v>
+        <v>60.5</v>
       </c>
       <c r="V43" s="2">
         <v>16.0</v>
@@ -4911,7 +4910,7 @@
         <v>115.0</v>
       </c>
       <c r="AK43" s="4">
-        <v>8.8</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="44">
@@ -4968,7 +4967,7 @@
         <v>3.0</v>
       </c>
       <c r="U44" s="4">
-        <v>55.9</v>
+        <v>60.5</v>
       </c>
       <c r="V44" s="2">
         <v>16.0</v>
@@ -5015,7 +5014,7 @@
         <v>54.0</v>
       </c>
       <c r="AK44" s="4">
-        <v>8.8</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="45">
@@ -5072,7 +5071,7 @@
         <v>3.0</v>
       </c>
       <c r="U45" s="4">
-        <v>55.9</v>
+        <v>60.5</v>
       </c>
       <c r="V45" s="2">
         <v>16.0</v>
@@ -5121,7 +5120,7 @@
         <v>52.0</v>
       </c>
       <c r="AK45" s="4">
-        <v>8.8</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="46">
@@ -5178,7 +5177,7 @@
         <v>2.5</v>
       </c>
       <c r="U46" s="4">
-        <v>48.8</v>
+        <v>52.8</v>
       </c>
       <c r="V46" s="2">
         <v>14.5</v>
@@ -5224,7 +5223,7 @@
         <v>36.0</v>
       </c>
       <c r="AK46" s="4">
-        <v>7.6</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="47">
@@ -5281,7 +5280,7 @@
         <v>3.0</v>
       </c>
       <c r="U47" s="4">
-        <v>48.8</v>
+        <v>52.8</v>
       </c>
       <c r="V47" s="2">
         <v>14.5</v>
@@ -5327,7 +5326,7 @@
         <v>53.0</v>
       </c>
       <c r="AK47" s="4">
-        <v>7.6</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="48">
@@ -5384,7 +5383,7 @@
         <v>3.5</v>
       </c>
       <c r="U48" s="4">
-        <v>48.8</v>
+        <v>52.8</v>
       </c>
       <c r="V48" s="2">
         <v>14.5</v>
@@ -5430,7 +5429,7 @@
         <v>77.0</v>
       </c>
       <c r="AK48" s="4">
-        <v>7.6</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="49">
@@ -5487,7 +5486,7 @@
         <v>2.5</v>
       </c>
       <c r="U49" s="4">
-        <v>55.9</v>
+        <v>70.2</v>
       </c>
       <c r="V49" s="2">
         <v>17.5</v>
@@ -5534,7 +5533,7 @@
         <v>55.0</v>
       </c>
       <c r="AK49" s="4">
-        <v>8.8</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="50">
@@ -5591,7 +5590,7 @@
         <v>3.0</v>
       </c>
       <c r="U50" s="4">
-        <v>55.9</v>
+        <v>70.2</v>
       </c>
       <c r="V50" s="2">
         <v>17.5</v>
@@ -5638,7 +5637,7 @@
         <v>55.0</v>
       </c>
       <c r="AK50" s="4">
-        <v>8.8</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="51">
@@ -5695,7 +5694,7 @@
         <v>3.5</v>
       </c>
       <c r="U51" s="4">
-        <v>55.9</v>
+        <v>70.2</v>
       </c>
       <c r="V51" s="2">
         <v>17.5</v>
@@ -5742,7 +5741,7 @@
         <v>58.0</v>
       </c>
       <c r="AK51" s="4">
-        <v>8.8</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="52">
@@ -5799,7 +5798,7 @@
         <v>3.0</v>
       </c>
       <c r="U52" s="4">
-        <v>64.7</v>
+        <v>60.5</v>
       </c>
       <c r="V52" s="2">
         <v>16.0</v>
@@ -5846,7 +5845,7 @@
         <v>40.0</v>
       </c>
       <c r="AK52" s="4">
-        <v>10.4</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="53">
@@ -5903,7 +5902,7 @@
         <v>3.0</v>
       </c>
       <c r="U53" s="4">
-        <v>64.7</v>
+        <v>60.5</v>
       </c>
       <c r="V53" s="2">
         <v>16.0</v>
@@ -5950,7 +5949,7 @@
         <v>62.0</v>
       </c>
       <c r="AK53" s="4">
-        <v>10.4</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="54">
@@ -6007,7 +6006,7 @@
         <v>3.0</v>
       </c>
       <c r="U54" s="4">
-        <v>64.7</v>
+        <v>60.5</v>
       </c>
       <c r="V54" s="2">
         <v>16.0</v>
@@ -6054,7 +6053,7 @@
         <v>90.0</v>
       </c>
       <c r="AK54" s="4">
-        <v>10.4</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="55">
@@ -6113,7 +6112,7 @@
         <v>2.0</v>
       </c>
       <c r="U55" s="4">
-        <v>59.2</v>
+        <v>62.4</v>
       </c>
       <c r="V55" s="2">
         <v>16.0</v>
@@ -6160,7 +6159,7 @@
         <v>36.0</v>
       </c>
       <c r="AK55" s="4">
-        <v>12.2</v>
+        <v>18.4</v>
       </c>
     </row>
     <row r="56">
@@ -6219,7 +6218,7 @@
         <v>2.5</v>
       </c>
       <c r="U56" s="4">
-        <v>59.2</v>
+        <v>62.5</v>
       </c>
       <c r="V56" s="2">
         <v>16.0</v>
@@ -6266,7 +6265,7 @@
         <v>38.0</v>
       </c>
       <c r="AK56" s="4">
-        <v>12.2</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="57">
@@ -6325,7 +6324,7 @@
         <v>3.0</v>
       </c>
       <c r="U57" s="4">
-        <v>59.3</v>
+        <v>62.5</v>
       </c>
       <c r="V57" s="2">
         <v>16.0</v>
@@ -6372,7 +6371,7 @@
         <v>61.0</v>
       </c>
       <c r="AK57" s="4">
-        <v>12.2</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="58">
@@ -6431,7 +6430,7 @@
         <v>3.5</v>
       </c>
       <c r="U58" s="4">
-        <v>59.2</v>
+        <v>62.5</v>
       </c>
       <c r="V58" s="2">
         <v>16.0</v>
@@ -6478,7 +6477,7 @@
         <v>92.0</v>
       </c>
       <c r="AK58" s="4">
-        <v>12.2</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="59">
@@ -6537,7 +6536,7 @@
         <v>4.0</v>
       </c>
       <c r="U59" s="4">
-        <v>59.2</v>
+        <v>62.5</v>
       </c>
       <c r="V59" s="2">
         <v>16.0</v>
@@ -6584,7 +6583,7 @@
         <v>130.0</v>
       </c>
       <c r="AK59" s="4">
-        <v>12.2</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="60">
@@ -6643,7 +6642,7 @@
         <v>3.0</v>
       </c>
       <c r="U60" s="4">
-        <v>59.3</v>
+        <v>62.5</v>
       </c>
       <c r="V60" s="2">
         <v>16.0</v>
@@ -6690,7 +6689,7 @@
         <v>59.0</v>
       </c>
       <c r="AK60" s="4">
-        <v>12.2</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="61">
@@ -6749,7 +6748,7 @@
         <v>3.0</v>
       </c>
       <c r="U61" s="4">
-        <v>59.3</v>
+        <v>62.5</v>
       </c>
       <c r="V61" s="2">
         <v>16.0</v>
@@ -6796,7 +6795,7 @@
         <v>60.0</v>
       </c>
       <c r="AK61" s="4">
-        <v>12.3</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="62">
@@ -6855,7 +6854,7 @@
         <v>3.0</v>
       </c>
       <c r="U62" s="4">
-        <v>59.3</v>
+        <v>62.5</v>
       </c>
       <c r="V62" s="2">
         <v>16.0</v>
@@ -6902,7 +6901,7 @@
         <v>58.0</v>
       </c>
       <c r="AK62" s="4">
-        <v>12.3</v>
+        <v>18.6</v>
       </c>
     </row>
     <row r="63">
@@ -6961,7 +6960,7 @@
         <v>3.0</v>
       </c>
       <c r="U63" s="4">
-        <v>59.3</v>
+        <v>62.5</v>
       </c>
       <c r="V63" s="2">
         <v>16.0</v>
@@ -7010,7 +7009,7 @@
         <v>54.0</v>
       </c>
       <c r="AK63" s="4">
-        <v>12.3</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="64">
@@ -7069,7 +7068,7 @@
         <v>2.5</v>
       </c>
       <c r="U64" s="4">
-        <v>50.2</v>
+        <v>52.8</v>
       </c>
       <c r="V64" s="2">
         <v>14.5</v>
@@ -7116,7 +7115,7 @@
         <v>38.0</v>
       </c>
       <c r="AK64" s="4">
-        <v>10.1</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="65">
@@ -7175,7 +7174,7 @@
         <v>3.0</v>
       </c>
       <c r="U65" s="4">
-        <v>50.2</v>
+        <v>52.8</v>
       </c>
       <c r="V65" s="2">
         <v>14.5</v>
@@ -7222,7 +7221,7 @@
         <v>58.0</v>
       </c>
       <c r="AK65" s="4">
-        <v>10.1</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="66">
@@ -7281,7 +7280,7 @@
         <v>3.5</v>
       </c>
       <c r="U66" s="4">
-        <v>50.2</v>
+        <v>52.8</v>
       </c>
       <c r="V66" s="2">
         <v>14.5</v>
@@ -7328,7 +7327,7 @@
         <v>84.0</v>
       </c>
       <c r="AK66" s="4">
-        <v>10.1</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="67">
@@ -7387,7 +7386,7 @@
         <v>2.5</v>
       </c>
       <c r="U67" s="4">
-        <v>68.4</v>
+        <v>72.2</v>
       </c>
       <c r="V67" s="2">
         <v>17.5</v>
@@ -7434,7 +7433,7 @@
         <v>43.0</v>
       </c>
       <c r="AK67" s="4">
-        <v>14.5</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="68">
@@ -7493,7 +7492,7 @@
         <v>3.0</v>
       </c>
       <c r="U68" s="4">
-        <v>68.4</v>
+        <v>72.2</v>
       </c>
       <c r="V68" s="2">
         <v>17.5</v>
@@ -7540,7 +7539,7 @@
         <v>68.0</v>
       </c>
       <c r="AK68" s="4">
-        <v>14.5</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="69">
@@ -7569,8 +7568,12 @@
       <c r="I69" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J69" s="6"/>
-      <c r="K69" s="6"/>
+      <c r="J69" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K69" s="8">
+        <v>215.7</v>
+      </c>
       <c r="L69" s="3">
         <v>0.0</v>
       </c>
@@ -7594,7 +7597,9 @@
       <c r="T69" s="1">
         <v>3.5</v>
       </c>
-      <c r="U69" s="3"/>
+      <c r="U69" s="4">
+        <v>72.1</v>
+      </c>
       <c r="V69" s="2">
         <v>17.5</v>
       </c>
@@ -7619,15 +7624,29 @@
         <f>0.36*8</f>
         <v>2.88</v>
       </c>
-      <c r="AC69" s="6"/>
+      <c r="AC69" s="8">
+        <v>2.0</v>
+      </c>
       <c r="AD69" s="6"/>
       <c r="AE69" s="6"/>
-      <c r="AF69" s="6"/>
-      <c r="AG69" s="6"/>
-      <c r="AH69" s="6"/>
-      <c r="AI69" s="6"/>
-      <c r="AJ69" s="6"/>
-      <c r="AK69" s="6"/>
+      <c r="AF69" s="8">
+        <v>2.9</v>
+      </c>
+      <c r="AG69" s="8">
+        <v>2.9</v>
+      </c>
+      <c r="AH69" s="8">
+        <v>5.8</v>
+      </c>
+      <c r="AI69" s="8">
+        <v>58.9</v>
+      </c>
+      <c r="AJ69" s="8">
+        <v>99.0</v>
+      </c>
+      <c r="AK69" s="4">
+        <v>21.8</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="3"/>
@@ -7683,7 +7702,7 @@
         <v>2.5</v>
       </c>
       <c r="U70" s="4">
-        <v>66.4</v>
+        <v>72.0</v>
       </c>
       <c r="V70" s="2">
         <v>17.5</v>
@@ -7727,7 +7746,7 @@
         <v>41.3</v>
       </c>
       <c r="AK70" s="4">
-        <v>10.6</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="71">
@@ -7784,7 +7803,7 @@
         <v>3.0</v>
       </c>
       <c r="U71" s="4">
-        <v>66.4</v>
+        <v>72.0</v>
       </c>
       <c r="V71" s="2">
         <v>17.5</v>
@@ -7828,7 +7847,7 @@
         <v>67.9</v>
       </c>
       <c r="AK71" s="4">
-        <v>10.6</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="72">
@@ -7885,7 +7904,7 @@
         <v>3.5</v>
       </c>
       <c r="U72" s="4">
-        <v>66.4</v>
+        <v>71.9</v>
       </c>
       <c r="V72" s="2">
         <v>17.5</v>
@@ -7929,7 +7948,7 @@
         <v>95.7</v>
       </c>
       <c r="AK72" s="4">
-        <v>10.6</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="73">
@@ -7986,7 +8005,7 @@
         <v>4.0</v>
       </c>
       <c r="U73" s="4">
-        <v>66.4</v>
+        <v>72.0</v>
       </c>
       <c r="V73" s="2">
         <v>17.5</v>
@@ -8030,7 +8049,7 @@
         <v>136.9</v>
       </c>
       <c r="AK73" s="4">
-        <v>10.6</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="74">
@@ -8087,7 +8106,7 @@
         <v>2.0</v>
       </c>
       <c r="U74" s="4">
-        <v>67.3</v>
+        <v>73.0</v>
       </c>
       <c r="V74" s="2">
         <v>17.5</v>
@@ -8131,7 +8150,7 @@
         <v>47.2</v>
       </c>
       <c r="AK74" s="4">
-        <v>10.8</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="75">

</xml_diff>